<commit_message>
begin diffcult multiple work.
</commit_message>
<xml_diff>
--- a/excel/bike_data.xlsx
+++ b/excel/bike_data.xlsx
@@ -1645,8 +1645,8 @@
   <sheetPr/>
   <dimension ref="A1:AL85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="Z12" sqref="Z12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -2313,7 +2313,7 @@
       <c r="O6" s="2">
         <v>1</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="5" t="s">
         <v>46</v>
       </c>
       <c r="Q6">
@@ -8577,7 +8577,7 @@
       <c r="O60" s="2">
         <v>1</v>
       </c>
-      <c r="P60" t="s">
+      <c r="P60" s="5" t="s">
         <v>153</v>
       </c>
       <c r="Q60">

</xml_diff>